<commit_message>
adding the final format
</commit_message>
<xml_diff>
--- a/world.xlsx
+++ b/world.xlsx
@@ -554,20 +554,36 @@
         <v>0</v>
       </c>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="3:12" ht="25" customHeight="1">
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="K3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="3:12">
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="3:12" ht="25" customHeight="1">
+      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12">
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
@@ -575,15 +591,17 @@
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="3:12">
       <c r="C6" s="2" t="s">
@@ -593,16 +611,16 @@
         <v>6</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="3:12">
@@ -613,30 +631,16 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12">
-      <c r="G8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="3">
+      <c r="L7" s="3">
         <v>1</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="3:12" ht="25" customHeight="1">
@@ -644,38 +648,44 @@
         <v>8</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="K9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" ht="25" customHeight="1">
+      <c r="G9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="K9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="3:12">
       <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="3:12" ht="25" customHeight="1">
+      <c r="G10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="K10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="3:12">
       <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="6"/>
       <c r="G11" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H11" s="6"/>
-      <c r="K11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" s="4"/>
+      <c r="K11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="3:12">
       <c r="C12" s="5" t="s">
@@ -685,13 +695,17 @@
         <v>13</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="K12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="3:12">
       <c r="C13" s="5" t="s">
@@ -701,15 +715,17 @@
         <v>15</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="3:12">
       <c r="C14" s="5" t="s">
@@ -719,16 +735,16 @@
         <v>17</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="3:12">
@@ -739,47 +755,25 @@
         <v>19</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="3:12">
-      <c r="G16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12">
-      <c r="K17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="3:12" ht="25" customHeight="1">
+    </row>
+    <row r="18" spans="3:4" ht="25" customHeight="1">
       <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="3:12">
+    <row r="19" spans="3:4">
       <c r="C19" s="5" t="s">
         <v>9</v>
       </c>
@@ -787,13 +781,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="3:12">
+    <row r="20" spans="3:4">
       <c r="C20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="3:12">
+    <row r="21" spans="3:4">
       <c r="C21" s="5" t="s">
         <v>12</v>
       </c>
@@ -801,7 +795,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="3:12">
+    <row r="22" spans="3:4">
       <c r="C22" s="5" t="s">
         <v>14</v>
       </c>
@@ -809,7 +803,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="3:12">
+    <row r="23" spans="3:4">
       <c r="C23" s="5" t="s">
         <v>16</v>
       </c>
@@ -817,7 +811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="3:12">
+    <row r="24" spans="3:4">
       <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
@@ -825,7 +819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="3:12">
+    <row r="27" spans="3:4">
       <c r="C27" s="5" t="s">
         <v>9</v>
       </c>
@@ -833,13 +827,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="3:12">
+    <row r="28" spans="3:4">
       <c r="C28" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="3:12">
+    <row r="29" spans="3:4">
       <c r="C29" s="5" t="s">
         <v>12</v>
       </c>
@@ -847,7 +841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="3:12">
+    <row r="30" spans="3:4">
       <c r="C30" s="5" t="s">
         <v>14</v>
       </c>
@@ -855,7 +849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="3:12">
+    <row r="31" spans="3:4">
       <c r="C31" s="5" t="s">
         <v>16</v>
       </c>
@@ -863,7 +857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="3:12">
+    <row r="32" spans="3:4">
       <c r="C32" s="5" t="s">
         <v>18</v>
       </c>
@@ -968,10 +962,10 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>